<commit_message>
fix: added research to spreadsheet
</commit_message>
<xml_diff>
--- a/Mappings/ChecklistPainBehavior - STU3.xlsx
+++ b/Mappings/ChecklistPainBehavior - STU3.xlsx
@@ -10,15 +10,16 @@
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
     <sheet name="Information Model" sheetId="3" r:id="rId3"/>
-    <sheet name="Data" sheetId="4" r:id="rId4"/>
-    <sheet name="Terms of Use" sheetId="5" r:id="rId5"/>
+    <sheet name="Research" sheetId="6" r:id="rId4"/>
+    <sheet name="Data" sheetId="4" r:id="rId5"/>
+    <sheet name="Terms of Use" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0" iterate="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="167">
   <si>
     <t>Subject</t>
   </si>
@@ -480,6 +481,51 @@
   </si>
   <si>
     <t>1 or 0. valuequantity might not be correct as, for example, 0,75 is also possible</t>
+  </si>
+  <si>
+    <t>Checkbox searched for existing profiles / implementation on:</t>
+  </si>
+  <si>
+    <t>Checkbox!</t>
+  </si>
+  <si>
+    <t>Searchwords</t>
+  </si>
+  <si>
+    <t>Found results:</t>
+  </si>
+  <si>
+    <t>HL7 FHIR Specification</t>
+  </si>
+  <si>
+    <t>HL7 FHIR profiles</t>
+  </si>
+  <si>
+    <t>no relevant</t>
+  </si>
+  <si>
+    <t>HL7 FHIR profiles - latest version latest version (build)</t>
+  </si>
+  <si>
+    <t>HL7 FHIR extension registry</t>
+  </si>
+  <si>
+    <t>HL7 FHIR extension registry - latest version (build)</t>
+  </si>
+  <si>
+    <t>HL7 FHIR implementation guides (e.g. Argonaut)</t>
+  </si>
+  <si>
+    <t>Simplifier.net</t>
+  </si>
+  <si>
+    <t>Zulip (chat.fhir.org)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Google </t>
+  </si>
+  <si>
+    <t>checklist pain behaviour</t>
   </si>
 </sst>
 </file>
@@ -640,13 +686,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,10 +1251,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="16"/>
     </row>
     <row r="3" spans="2:3">
       <c r="B3" s="2" t="s">
@@ -1416,9 +1462,109 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>163</v>
+      </c>
+      <c r="C8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" t="s">
+        <v>166</v>
+      </c>
+      <c r="F9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" t="s">
+        <v>166</v>
+      </c>
+      <c r="F10" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
@@ -1546,10 +1692,10 @@
         <v>82</v>
       </c>
       <c r="N4" s="2"/>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="14" t="s">
         <v>146</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="P4" s="15" t="s">
         <v>150</v>
       </c>
       <c r="Q4" s="2"/>
@@ -1586,11 +1732,11 @@
         <v>87</v>
       </c>
       <c r="N5" s="2"/>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="15" t="s">
+      <c r="P5" s="15"/>
+      <c r="Q5" s="14" t="s">
         <v>151</v>
       </c>
       <c r="R5" s="2"/>
@@ -1624,10 +1770,10 @@
         <v>91</v>
       </c>
       <c r="N6" s="2"/>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="P6" s="16"/>
+      <c r="P6" s="15"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
@@ -1660,10 +1806,10 @@
         <v>95</v>
       </c>
       <c r="N7" s="2"/>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="P7" s="16"/>
+      <c r="P7" s="15"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
@@ -1696,10 +1842,10 @@
         <v>99</v>
       </c>
       <c r="N8" s="2"/>
-      <c r="O8" s="15" t="s">
+      <c r="O8" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="P8" s="16"/>
+      <c r="P8" s="15"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
@@ -1732,10 +1878,10 @@
         <v>103</v>
       </c>
       <c r="N9" s="2"/>
-      <c r="O9" s="15" t="s">
+      <c r="O9" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="P9" s="16"/>
+      <c r="P9" s="15"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
@@ -1768,10 +1914,10 @@
         <v>107</v>
       </c>
       <c r="N10" s="2"/>
-      <c r="O10" s="15" t="s">
+      <c r="O10" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="P10" s="16"/>
+      <c r="P10" s="15"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
@@ -1804,10 +1950,10 @@
         <v>111</v>
       </c>
       <c r="N11" s="2"/>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="P11" s="16"/>
+      <c r="P11" s="15"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
@@ -1840,10 +1986,10 @@
         <v>115</v>
       </c>
       <c r="N12" s="2"/>
-      <c r="O12" s="15" t="s">
+      <c r="O12" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="P12" s="16"/>
+      <c r="P12" s="15"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
@@ -1876,10 +2022,10 @@
         <v>119</v>
       </c>
       <c r="N13" s="2"/>
-      <c r="O13" s="15" t="s">
+      <c r="O13" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="P13" s="16"/>
+      <c r="P13" s="15"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
@@ -1912,10 +2058,10 @@
         <v>123</v>
       </c>
       <c r="N14" s="2"/>
-      <c r="O14" s="15" t="s">
+      <c r="O14" s="14" t="s">
         <v>147</v>
       </c>
-      <c r="P14" s="16"/>
+      <c r="P14" s="15"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
@@ -1948,10 +2094,10 @@
         <v>129</v>
       </c>
       <c r="N15" s="2"/>
-      <c r="O15" s="15" t="s">
+      <c r="O15" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="P15" s="16" t="s">
+      <c r="P15" s="15" t="s">
         <v>150</v>
       </c>
       <c r="Q15" s="2"/>
@@ -1988,10 +2134,10 @@
       <c r="N16" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="O16" s="15" t="s">
+      <c r="O16" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="P16" s="16" t="s">
+      <c r="P16" s="15" t="s">
         <v>150</v>
       </c>
       <c r="Q16" s="2"/>
@@ -2006,7 +2152,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B7"/>
   <sheetViews>

</xml_diff>

<commit_message>
fix: added research to spreadsheet - 2
</commit_message>
<xml_diff>
--- a/Mappings/ChecklistPainBehavior - STU3.xlsx
+++ b/Mappings/ChecklistPainBehavior - STU3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13740" activeTab="3"/>
+    <workbookView xWindow="630" yWindow="630" windowWidth="27495" windowHeight="13740" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="168">
   <si>
     <t>Subject</t>
   </si>
@@ -526,6 +526,9 @@
   </si>
   <si>
     <t>checklist pain behaviour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"" </t>
   </si>
 </sst>
 </file>
@@ -1464,7 +1467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -1564,8 +1567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S16"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1774,7 +1777,9 @@
         <v>147</v>
       </c>
       <c r="P6" s="15"/>
-      <c r="Q6" s="2"/>
+      <c r="Q6" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
     </row>
@@ -1810,7 +1815,9 @@
         <v>147</v>
       </c>
       <c r="P7" s="15"/>
-      <c r="Q7" s="2"/>
+      <c r="Q7" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
     </row>
@@ -1846,7 +1853,9 @@
         <v>147</v>
       </c>
       <c r="P8" s="15"/>
-      <c r="Q8" s="2"/>
+      <c r="Q8" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
     </row>
@@ -1882,7 +1891,9 @@
         <v>147</v>
       </c>
       <c r="P9" s="15"/>
-      <c r="Q9" s="2"/>
+      <c r="Q9" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
     </row>
@@ -1918,7 +1929,9 @@
         <v>147</v>
       </c>
       <c r="P10" s="15"/>
-      <c r="Q10" s="2"/>
+      <c r="Q10" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
     </row>
@@ -1954,7 +1967,9 @@
         <v>147</v>
       </c>
       <c r="P11" s="15"/>
-      <c r="Q11" s="2"/>
+      <c r="Q11" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
     </row>
@@ -1990,7 +2005,9 @@
         <v>147</v>
       </c>
       <c r="P12" s="15"/>
-      <c r="Q12" s="2"/>
+      <c r="Q12" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
     </row>
@@ -2026,7 +2043,9 @@
         <v>147</v>
       </c>
       <c r="P13" s="15"/>
-      <c r="Q13" s="2"/>
+      <c r="Q13" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
     </row>
@@ -2062,7 +2081,9 @@
         <v>147</v>
       </c>
       <c r="P14" s="15"/>
-      <c r="Q14" s="2"/>
+      <c r="Q14" s="2" t="s">
+        <v>167</v>
+      </c>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
     </row>

</xml_diff>